<commit_message>
revised and renumbered use cases. requirements doc nearly completed. RTM document has been revised.
</commit_message>
<xml_diff>
--- a/documents/CouponLoyaltyRTM.xlsx
+++ b/documents/CouponLoyaltyRTM.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
   <si>
     <t>Entry #</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>Type (see Definitions tab)</t>
-  </si>
-  <si>
-    <t>A Customer Marketing Report shall be produced by the application, on demand.</t>
   </si>
   <si>
     <t>Definitions</t>
@@ -151,50 +148,77 @@
     <t>Use Case Name</t>
   </si>
   <si>
-    <t>UC2_Personnel_Services_Tracking_Report</t>
-  </si>
-  <si>
-    <t>UC3_Service_Date_Report</t>
-  </si>
-  <si>
-    <t>UC4_Customer_Invoice_Report</t>
-  </si>
-  <si>
-    <t>UC5_Billing_Entry_Screen</t>
-  </si>
-  <si>
-    <t>UC6_Customer_Marketing_Report</t>
-  </si>
-  <si>
     <t xml:space="preserve">A loyalty program system that uses the user's credit card, phone number, or email to create a unique ID. </t>
   </si>
   <si>
-    <t xml:space="preserve">Web interface has the capability of pushing coupons, creating coupon discounts, selecting certain items, discount base on category, specific items, or all items) </t>
-  </si>
-  <si>
-    <t>A database that is able to store all necessary information such as sales, cost, reports, and inventory spacing</t>
-  </si>
-  <si>
     <t>Mama G's General Store Application: Requirements Traceability Matrix</t>
   </si>
   <si>
-    <t>UC1_Loyalty_Tracking_System</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A web interface that can generate reports on demand by selecting a drop down menu. 3(Most Frequent buyer, Least Frequent buyer, Everybody) x 5(Date Range, Season range, Weekends,  weekdays, All days) x 3(Highest Volume, Lowest Volume, All Volume) permuation will be provide for flexible select and 5 default recommend (will provide example later) </t>
-  </si>
-  <si>
     <t>Generate report of used coupon report ratio on web interface on demand</t>
   </si>
   <si>
-    <t>SW, DR</t>
+    <t>Users, both employees and the store owner, need to be able to log into the system</t>
+  </si>
+  <si>
+    <t>UC1_User_Login</t>
+  </si>
+  <si>
+    <t>SW,DR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC2_Loyalty_Tracking_System: </t>
+  </si>
+  <si>
+    <t>A web interface that can generate sales reports on demand.</t>
+  </si>
+  <si>
+    <t>UC3_View_Sales_Report</t>
+  </si>
+  <si>
+    <t>UC4_Customer_Absent_Report</t>
+  </si>
+  <si>
+    <t>A report on the customers who have not bought anything in the past 90 days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC5_Coupon_Ratio_Report </t>
+  </si>
+  <si>
+    <t>A way to manually generate coupons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC6_Create_Coupon </t>
+  </si>
+  <si>
+    <t>A way to view all available coupons</t>
+  </si>
+  <si>
+    <t>UC7_View_Available_Coupons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC8_Sales_Summary_Report </t>
+  </si>
+  <si>
+    <t>UC9_Frequent_Buyer_Report</t>
+  </si>
+  <si>
+    <t>A way for all users to be able to change their password</t>
+  </si>
+  <si>
+    <t>UC10_Change_Password</t>
+  </si>
+  <si>
+    <t>A way to generate sales reports to understand sales trends</t>
+  </si>
+  <si>
+    <t>A way to report on frequent buyers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,6 +239,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -244,7 +274,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -332,6 +362,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -365,9 +410,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -379,22 +421,25 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -700,10 +745,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -717,172 +762,228 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25">
-      <c r="A1" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
+      <c r="A1" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="25.5" customHeight="1">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="16" customFormat="1" ht="18">
+      <c r="A3" s="25">
+        <v>1</v>
+      </c>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="16" customFormat="1" ht="36">
+      <c r="A4" s="26">
+        <v>2</v>
+      </c>
+      <c r="B4" s="26">
+        <v>2</v>
+      </c>
+      <c r="C4" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="16" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A3" s="18">
-        <v>1</v>
-      </c>
-      <c r="B3" s="18">
-        <v>2</v>
-      </c>
-      <c r="C3" s="17" t="s">
+      <c r="D4" s="27" t="s">
         <v>47</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="F3" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="16" customFormat="1" ht="56">
-      <c r="A4" s="23">
-        <v>2</v>
-      </c>
-      <c r="B4" s="23">
-        <v>2</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>42</v>
       </c>
       <c r="E4" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="16" customFormat="1" ht="18">
+      <c r="A5" s="25">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" s="16" customFormat="1" ht="28">
-      <c r="A5" s="18">
-        <v>3</v>
-      </c>
-      <c r="B5" s="18">
+      <c r="B5" s="25">
         <v>2</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="17" t="s">
-        <v>43</v>
+      <c r="D5" s="28" t="s">
+        <v>49</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" s="18">
+        <v>19</v>
+      </c>
+      <c r="F5" s="25">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="16" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A6" s="23">
+    <row r="6" spans="1:8" s="16" customFormat="1" ht="18">
+      <c r="A6" s="26">
         <v>4</v>
       </c>
-      <c r="B6" s="23">
-        <v>3</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>44</v>
+      <c r="B6" s="26">
+        <v>2</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>50</v>
       </c>
       <c r="E6" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="26">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="16" customFormat="1" ht="35.25" customHeight="1">
-      <c r="A7" s="18">
+    <row r="7" spans="1:8" s="16" customFormat="1" ht="18">
+      <c r="A7" s="25">
         <v>5</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="25">
         <v>3</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>45</v>
+      <c r="C7" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>52</v>
       </c>
       <c r="E7" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="16" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A8" s="23">
+      <c r="F7" s="25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="16" customFormat="1" ht="18">
+      <c r="A8" s="26">
         <v>6</v>
       </c>
-      <c r="B8" s="23">
-        <v>3</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="24" t="s">
+      <c r="B8" s="26"/>
+      <c r="C8" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="F8" s="26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="16" customFormat="1" ht="24.75" customHeight="1">
+      <c r="A9" s="25">
+        <v>7</v>
+      </c>
+      <c r="B9" s="25"/>
+      <c r="C9" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="16" customFormat="1" ht="18">
+      <c r="A10" s="26">
+        <v>8</v>
+      </c>
+      <c r="B10" s="26">
+        <v>5</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="23">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="16" customFormat="1" ht="36" customHeight="1">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="18"/>
-    </row>
-    <row r="10" spans="1:8" s="16" customFormat="1" ht="37.5" customHeight="1">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="23"/>
+      <c r="F10" s="26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="16" customFormat="1" ht="18">
+      <c r="A11" s="25">
+        <v>9</v>
+      </c>
+      <c r="B11" s="25">
+        <v>4</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="18">
+      <c r="A12" s="26">
+        <v>10</v>
+      </c>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="26">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -912,12 +1013,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="24"/>
       <c r="C1" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="16" customFormat="1" ht="42">
@@ -928,18 +1029,18 @@
         <v>21</v>
       </c>
       <c r="C2" s="17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="16" customFormat="1">
+      <c r="A3" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="16" customFormat="1">
-      <c r="A3" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="16" customFormat="1">
@@ -950,18 +1051,18 @@
         <v>23</v>
       </c>
       <c r="C4" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="16" customFormat="1" ht="28">
+      <c r="A5" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="22" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="16" customFormat="1" ht="28">
-      <c r="A5" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="16" customFormat="1">
@@ -972,18 +1073,18 @@
         <v>25</v>
       </c>
       <c r="C6" s="17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="16" customFormat="1" ht="42">
+      <c r="A7" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="22" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="16" customFormat="1" ht="42">
-      <c r="A7" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="16" customFormat="1">
@@ -994,7 +1095,7 @@
         <v>27</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="16" customFormat="1">

</xml_diff>

<commit_message>
Updated the RTM, use cases, and the overall spec document.
</commit_message>
<xml_diff>
--- a/documents/CouponLoyaltyRTM.xlsx
+++ b/documents/CouponLoyaltyRTM.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mwoodie3/git-work/csc4370/documents/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="700" yWindow="460" windowWidth="25980" windowHeight="14640"/>
+    <workbookView xWindow="2620" yWindow="1380" windowWidth="25980" windowHeight="14640"/>
   </bookViews>
   <sheets>
     <sheet name="RTM" sheetId="1" r:id="rId1"/>
@@ -148,9 +153,6 @@
     <t>Use Case Name</t>
   </si>
   <si>
-    <t xml:space="preserve">A loyalty program system that uses the user's credit card, phone number, or email to create a unique ID. </t>
-  </si>
-  <si>
     <t>Mama G's General Store Application: Requirements Traceability Matrix</t>
   </si>
   <si>
@@ -166,9 +168,6 @@
     <t>SW,DR</t>
   </si>
   <si>
-    <t xml:space="preserve">UC2_Loyalty_Tracking_System: </t>
-  </si>
-  <si>
     <t>A web interface that can generate sales reports on demand.</t>
   </si>
   <si>
@@ -196,9 +195,6 @@
     <t>UC7_View_Available_Coupons</t>
   </si>
   <si>
-    <t xml:space="preserve">UC8_Sales_Summary_Report </t>
-  </si>
-  <si>
     <t>UC9_Frequent_Buyer_Report</t>
   </si>
   <si>
@@ -208,10 +204,19 @@
     <t>UC10_Change_Password</t>
   </si>
   <si>
-    <t>A way to generate sales reports to understand sales trends</t>
-  </si>
-  <si>
     <t>A way to report on frequent buyers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A loyalty program system that uses the user's phone number, or email to create a unique ID. </t>
+  </si>
+  <si>
+    <t>A way for users to generate reports and filter on date, product, etc.</t>
+  </si>
+  <si>
+    <t>UC8_Generate_Report</t>
+  </si>
+  <si>
+    <t>UC2_Loyalty_Tracking_System:</t>
   </si>
 </sst>
 </file>
@@ -423,12 +428,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -440,6 +439,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -748,10 +753,10 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" style="2" customWidth="1"/>
@@ -761,19 +766,19 @@
     <col min="6" max="6" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="25">
-      <c r="A1" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
+    <row r="1" spans="1:8" ht="26" x14ac:dyDescent="0.2">
+      <c r="A1" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="25.5" customHeight="1">
+    <row r="2" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
@@ -793,196 +798,202 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="16" customFormat="1" ht="18">
-      <c r="A3" s="25">
+    <row r="3" spans="1:8" s="16" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+      <c r="A3" s="23">
         <v>1</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25" t="s">
+      <c r="B3" s="23">
+        <v>3</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="E3" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="F3" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="16" customFormat="1" ht="38" x14ac:dyDescent="0.2">
+      <c r="A4" s="24">
+        <v>2</v>
+      </c>
+      <c r="B4" s="24">
+        <v>2</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="16" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+      <c r="A5" s="23">
+        <v>3</v>
+      </c>
+      <c r="B5" s="23">
+        <v>2</v>
+      </c>
+      <c r="C5" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="25">
+      <c r="D5" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="16" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+      <c r="A6" s="24">
+        <v>4</v>
+      </c>
+      <c r="B6" s="24">
+        <v>2</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="24">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="16" customFormat="1" ht="36">
-      <c r="A4" s="26">
-        <v>2</v>
-      </c>
-      <c r="B4" s="26">
-        <v>2</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="26" t="s">
+    <row r="7" spans="1:8" s="16" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+      <c r="A7" s="23">
+        <v>5</v>
+      </c>
+      <c r="B7" s="23">
+        <v>3</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="26">
+      <c r="F7" s="23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="16" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+      <c r="A8" s="24">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" s="16" customFormat="1" ht="18">
-      <c r="A5" s="25">
-        <v>3</v>
-      </c>
-      <c r="B5" s="25">
-        <v>2</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="25" t="s">
+      <c r="B8" s="24">
+        <v>4</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="16" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="23">
+        <v>7</v>
+      </c>
+      <c r="B9" s="23">
+        <v>4</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="16" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+      <c r="A10" s="24">
+        <v>8</v>
+      </c>
+      <c r="B10" s="24">
+        <v>5</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F10" s="24">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="16" customFormat="1" ht="18">
-      <c r="A6" s="26">
+    <row r="11" spans="1:8" s="16" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+      <c r="A11" s="23">
+        <v>9</v>
+      </c>
+      <c r="B11" s="23">
         <v>4</v>
       </c>
-      <c r="B6" s="26">
-        <v>2</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="26" t="s">
+      <c r="C11" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="26">
+      <c r="F11" s="23">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="16" customFormat="1" ht="18">
-      <c r="A7" s="25">
-        <v>5</v>
-      </c>
-      <c r="B7" s="25">
-        <v>3</v>
-      </c>
-      <c r="C7" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="16" customFormat="1" ht="18">
-      <c r="A8" s="26">
-        <v>6</v>
-      </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" s="26">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="16" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A9" s="25">
-        <v>7</v>
-      </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="28" t="s">
+    <row r="12" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A12" s="24">
+        <v>10</v>
+      </c>
+      <c r="B12" s="24"/>
+      <c r="C12" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" s="25">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="16" customFormat="1" ht="18">
-      <c r="A10" s="26">
-        <v>8</v>
-      </c>
-      <c r="B10" s="26">
-        <v>5</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" s="27" t="s">
+      <c r="D12" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="26">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="16" customFormat="1" ht="18">
-      <c r="A11" s="25">
-        <v>9</v>
-      </c>
-      <c r="B11" s="25">
-        <v>4</v>
-      </c>
-      <c r="C11" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="25">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="18">
-      <c r="A12" s="26">
+      <c r="E12" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="24">
         <v>10</v>
-      </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="26">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -990,11 +1001,6 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1006,22 +1012,22 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="37.5" customWidth="1"/>
     <col min="3" max="3" width="78.33203125" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="24"/>
+      <c r="B1" s="28"/>
       <c r="C1" s="14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="16" customFormat="1" ht="42">
+    <row r="2" spans="1:3" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>15</v>
       </c>
@@ -1032,7 +1038,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="16" customFormat="1">
+    <row r="3" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
         <v>16</v>
       </c>
@@ -1043,7 +1049,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="16" customFormat="1">
+    <row r="4" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>17</v>
       </c>
@@ -1054,7 +1060,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="16" customFormat="1" ht="28">
+    <row r="5" spans="1:3" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
         <v>18</v>
       </c>
@@ -1065,7 +1071,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="16" customFormat="1">
+    <row r="6" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>19</v>
       </c>
@@ -1076,7 +1082,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="16" customFormat="1" ht="42">
+    <row r="7" spans="1:3" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
         <v>20</v>
       </c>
@@ -1087,7 +1093,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="16" customFormat="1">
+    <row r="8" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
         <v>28</v>
       </c>
@@ -1098,7 +1104,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="16" customFormat="1">
+    <row r="9" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C9" s="17"/>
     </row>
   </sheetData>
@@ -1106,11 +1112,6 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1122,13 +1123,13 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="26.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:16">
+    <row r="3" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C3" s="3"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -1144,7 +1145,7 @@
       <c r="O3" s="4"/>
       <c r="P3" s="5"/>
     </row>
-    <row r="4" spans="3:16">
+    <row r="4" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C4" s="6" t="s">
         <v>3</v>
       </c>
@@ -1162,7 +1163,7 @@
       <c r="O4" s="7"/>
       <c r="P4" s="8"/>
     </row>
-    <row r="5" spans="3:16">
+    <row r="5" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C5" s="6"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
@@ -1178,7 +1179,7 @@
       <c r="O5" s="7"/>
       <c r="P5" s="8"/>
     </row>
-    <row r="6" spans="3:16">
+    <row r="6" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C6" s="6" t="s">
         <v>4</v>
       </c>
@@ -1196,7 +1197,7 @@
       <c r="O6" s="7"/>
       <c r="P6" s="8"/>
     </row>
-    <row r="7" spans="3:16">
+    <row r="7" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C7" s="6" t="s">
         <v>5</v>
       </c>
@@ -1226,7 +1227,7 @@
       <c r="O7" s="7"/>
       <c r="P7" s="8"/>
     </row>
-    <row r="8" spans="3:16">
+    <row r="8" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C8" s="6"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
@@ -1242,7 +1243,7 @@
       <c r="O8" s="7"/>
       <c r="P8" s="8"/>
     </row>
-    <row r="9" spans="3:16">
+    <row r="9" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C9" s="6"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
@@ -1258,7 +1259,7 @@
       <c r="O9" s="7"/>
       <c r="P9" s="8"/>
     </row>
-    <row r="10" spans="3:16">
+    <row r="10" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C10" s="6" t="s">
         <v>13</v>
       </c>
@@ -1276,7 +1277,7 @@
       <c r="O10" s="7"/>
       <c r="P10" s="8"/>
     </row>
-    <row r="11" spans="3:16">
+    <row r="11" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C11" s="13">
         <v>41305</v>
       </c>
@@ -1296,7 +1297,7 @@
       <c r="O11" s="7"/>
       <c r="P11" s="8"/>
     </row>
-    <row r="12" spans="3:16">
+    <row r="12" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C12" s="6"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -1312,7 +1313,7 @@
       <c r="O12" s="7"/>
       <c r="P12" s="8"/>
     </row>
-    <row r="13" spans="3:16">
+    <row r="13" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C13" s="6"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -1328,7 +1329,7 @@
       <c r="O13" s="7"/>
       <c r="P13" s="8"/>
     </row>
-    <row r="14" spans="3:16">
+    <row r="14" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C14" s="6" t="s">
         <v>29</v>
       </c>
@@ -1346,7 +1347,7 @@
       <c r="O14" s="7"/>
       <c r="P14" s="8"/>
     </row>
-    <row r="15" spans="3:16">
+    <row r="15" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C15" s="6"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -1362,7 +1363,7 @@
       <c r="O15" s="7"/>
       <c r="P15" s="8"/>
     </row>
-    <row r="16" spans="3:16">
+    <row r="16" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C16" s="6"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
@@ -1378,7 +1379,7 @@
       <c r="O16" s="7"/>
       <c r="P16" s="8"/>
     </row>
-    <row r="17" spans="3:16">
+    <row r="17" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C17" s="6"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
@@ -1394,7 +1395,7 @@
       <c r="O17" s="7"/>
       <c r="P17" s="8"/>
     </row>
-    <row r="18" spans="3:16">
+    <row r="18" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C18" s="6"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
@@ -1410,7 +1411,7 @@
       <c r="O18" s="7"/>
       <c r="P18" s="8"/>
     </row>
-    <row r="19" spans="3:16">
+    <row r="19" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C19" s="6"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
@@ -1426,7 +1427,7 @@
       <c r="O19" s="7"/>
       <c r="P19" s="8"/>
     </row>
-    <row r="20" spans="3:16">
+    <row r="20" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C20" s="6"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
@@ -1442,7 +1443,7 @@
       <c r="O20" s="7"/>
       <c r="P20" s="8"/>
     </row>
-    <row r="21" spans="3:16">
+    <row r="21" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C21" s="6"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
@@ -1458,7 +1459,7 @@
       <c r="O21" s="7"/>
       <c r="P21" s="8"/>
     </row>
-    <row r="22" spans="3:16">
+    <row r="22" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C22" s="6"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
@@ -1474,7 +1475,7 @@
       <c r="O22" s="7"/>
       <c r="P22" s="8"/>
     </row>
-    <row r="23" spans="3:16">
+    <row r="23" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C23" s="6"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
@@ -1490,7 +1491,7 @@
       <c r="O23" s="7"/>
       <c r="P23" s="8"/>
     </row>
-    <row r="24" spans="3:16">
+    <row r="24" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C24" s="6"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
@@ -1506,7 +1507,7 @@
       <c r="O24" s="7"/>
       <c r="P24" s="8"/>
     </row>
-    <row r="25" spans="3:16">
+    <row r="25" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C25" s="6"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
@@ -1522,7 +1523,7 @@
       <c r="O25" s="7"/>
       <c r="P25" s="8"/>
     </row>
-    <row r="26" spans="3:16">
+    <row r="26" spans="3:16" x14ac:dyDescent="0.2">
       <c r="C26" s="9"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
@@ -1540,10 +1541,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>